<commit_message>
Actualización de avances en el cronograma
</commit_message>
<xml_diff>
--- a/01 Documentos/Cronograma/MS_CP.xlsx
+++ b/01 Documentos/Cronograma/MS_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvrui\Desktop\UNMSM\CICLO V\Gestión_Configuración\MedidaShoes\DevSoftAll\01 Documentos\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E206634-E81E-4CD9-8610-784FAD08762D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F84E58-1B63-42B5-9A62-723F996B6C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,20 +826,19 @@
     <xf numFmtId="164" fontId="1" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -851,22 +850,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,132 +1104,132 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="27">
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="38">
         <v>1</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="27" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="28">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="33">
         <v>44699</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="28">
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="33">
         <v>44778</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
       <c r="L10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1254,24 +1254,24 @@
       <c r="AA10" s="1"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="7">
         <v>44699</v>
       </c>
@@ -1284,24 +1284,24 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="8">
         <f t="shared" ref="L12:M12" si="0">L11</f>
         <v>44699</v>
@@ -1315,24 +1315,24 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
       <c r="L13" s="8">
         <f>L12</f>
         <v>44699</v>
@@ -1345,24 +1345,24 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="7">
         <v>44699</v>
       </c>
@@ -1375,24 +1375,24 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
       <c r="L15" s="8">
         <f>M14</f>
         <v>44703</v>
@@ -1405,24 +1405,24 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="7">
         <v>44706</v>
       </c>
@@ -1434,24 +1434,24 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="7">
         <f t="shared" ref="L17:M17" si="1">L16</f>
         <v>44706</v>
@@ -1461,28 +1461,28 @@
         <v>44715</v>
       </c>
       <c r="N17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
       <c r="L18" s="7">
         <f>L17</f>
         <v>44706</v>
@@ -1495,24 +1495,24 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="7">
         <v>44713</v>
       </c>
@@ -1524,24 +1524,24 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
       <c r="L20" s="7">
         <v>44713</v>
       </c>
@@ -1553,24 +1553,24 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
       <c r="L21" s="7">
         <v>44723</v>
       </c>
@@ -1582,24 +1582,24 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
       <c r="L22" s="7">
         <v>44729</v>
       </c>
@@ -1611,24 +1611,24 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
       <c r="L23" s="7">
         <v>44734</v>
       </c>
@@ -1640,18 +1640,18 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
       <c r="L24" s="12">
         <f>L11</f>
         <v>44699</v>
@@ -1662,28 +1662,28 @@
       </c>
       <c r="N24" s="13">
         <f>AVERAGE(N11:N23)</f>
-        <v>0.61538461538461542</v>
+        <v>0.69230769230769229</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="23"/>
       <c r="L25" s="8">
         <f>M24</f>
         <v>44736</v>
@@ -1696,24 +1696,24 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
       <c r="L26" s="7">
         <v>44736</v>
       </c>
@@ -1725,24 +1725,24 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="7">
         <v>44736</v>
       </c>
@@ -1754,24 +1754,24 @@
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="5" t="s">
         <v>67</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
       <c r="L28" s="7">
         <v>44736</v>
       </c>
@@ -1783,24 +1783,24 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="5" t="s">
         <v>70</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="23"/>
       <c r="L29" s="7">
         <v>44736</v>
       </c>
@@ -1812,24 +1812,24 @@
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="23"/>
       <c r="L30" s="7">
         <v>44748</v>
       </c>
@@ -1841,24 +1841,24 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="23"/>
       <c r="L31" s="7">
         <v>44755</v>
       </c>
@@ -1871,18 +1871,18 @@
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="23"/>
       <c r="L32" s="12">
         <f>L25</f>
         <v>44736</v>
@@ -1896,24 +1896,24 @@
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="23"/>
       <c r="L33" s="8">
         <f>M32</f>
         <v>44757</v>
@@ -1926,24 +1926,24 @@
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="23"/>
       <c r="L34" s="7">
         <v>44757</v>
       </c>
@@ -1955,24 +1955,24 @@
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
       <c r="L35" s="7">
         <v>44757</v>
       </c>
@@ -1984,24 +1984,24 @@
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="23"/>
       <c r="L36" s="7">
         <v>44757</v>
       </c>
@@ -2013,24 +2013,24 @@
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="23"/>
       <c r="L37" s="7">
         <v>44757</v>
       </c>
@@ -2042,24 +2042,24 @@
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="23"/>
       <c r="L38" s="7">
         <v>44762</v>
       </c>
@@ -2071,24 +2071,24 @@
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="23"/>
       <c r="L39" s="7">
         <v>44762</v>
       </c>
@@ -2100,24 +2100,24 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="23"/>
       <c r="L40" s="7">
         <v>44764</v>
       </c>
@@ -2129,24 +2129,24 @@
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="23"/>
       <c r="L41" s="7">
         <v>44769</v>
       </c>
@@ -2158,24 +2158,24 @@
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="23"/>
       <c r="L42" s="7">
         <v>44769</v>
       </c>
@@ -2187,24 +2187,24 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="23"/>
       <c r="L43" s="7">
         <v>44777</v>
       </c>
@@ -2216,24 +2216,24 @@
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="5" t="s">
         <v>100</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="23"/>
       <c r="L44" s="7">
         <v>44777</v>
       </c>
@@ -2245,18 +2245,18 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="29"/>
       <c r="F45" s="15"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="37"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="29"/>
       <c r="L45" s="17">
         <f>L33</f>
         <v>44757</v>
@@ -2270,14 +2270,14 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G47" s="1"/>
@@ -5146,6 +5146,77 @@
     </row>
   </sheetData>
   <mergeCells count="87">
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H40:K40"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B31:E31"/>
@@ -5162,77 +5233,6 @@
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B41:E41"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5253,120 +5253,120 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="43" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="43" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="43" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="43" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="43" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="43" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="43" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="43" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="43" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F11" s="2"/>
@@ -5392,6 +5392,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:H10"/>
@@ -5407,13 +5414,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Eliminar MS_CP de Desarrollo
</commit_message>
<xml_diff>
--- a/01 Documentos/Cronograma/MS_CP.xlsx
+++ b/01 Documentos/Cronograma/MS_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvrui\Desktop\UNMSM\CICLO V\Gestión_Configuración\MedidaShoes\DevSoftAll\01 Documentos\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D2D2F4-D44C-4305-8756-49AA5C72DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C3128B-0759-4768-960C-3BEBB9D06CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,19 +826,19 @@
     <xf numFmtId="164" fontId="1" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -850,23 +850,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:K17"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1104,132 +1104,132 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="40" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="38">
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="26">
         <v>1</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="38" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="38" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="33">
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="27">
         <v>44699</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="33">
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="27">
         <v>44778</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1254,24 +1254,24 @@
       <c r="AA10" s="1"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="7">
         <v>44699</v>
       </c>
@@ -1284,24 +1284,24 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="8">
         <f t="shared" ref="L12:M12" si="0">L11</f>
         <v>44699</v>
@@ -1315,24 +1315,24 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="8">
         <f>L12</f>
         <v>44699</v>
@@ -1345,24 +1345,24 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="7">
         <v>44699</v>
       </c>
@@ -1375,24 +1375,24 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="23"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="8">
         <f>M14</f>
         <v>44703</v>
@@ -1405,24 +1405,24 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="23"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="7">
         <v>44706</v>
       </c>
@@ -1434,24 +1434,24 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="23"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="7">
         <f t="shared" ref="L17:M17" si="1">L16</f>
         <v>44706</v>
@@ -1465,24 +1465,24 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="23"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
       <c r="L18" s="7">
         <f>L17</f>
         <v>44706</v>
@@ -1495,24 +1495,24 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="23"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="7">
         <v>44713</v>
       </c>
@@ -1524,24 +1524,24 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="23"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="7">
         <v>44713</v>
       </c>
@@ -1553,24 +1553,24 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="23"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="7">
         <v>44723</v>
       </c>
@@ -1578,28 +1578,28 @@
         <v>44729</v>
       </c>
       <c r="N21" s="9">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="23"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="7">
         <v>44729</v>
       </c>
@@ -1611,24 +1611,24 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="23"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="7">
         <v>44734</v>
       </c>
@@ -1640,18 +1640,18 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="23"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="12">
         <f>L11</f>
         <v>44699</v>
@@ -1662,28 +1662,28 @@
       </c>
       <c r="N24" s="13">
         <f>AVERAGE(N11:N23)</f>
-        <v>0.8</v>
+        <v>0.83076923076923082</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="23"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
       <c r="L25" s="8">
         <f>M24</f>
         <v>44736</v>
@@ -1696,24 +1696,24 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="23"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
       <c r="L26" s="7">
         <v>44736</v>
       </c>
@@ -1725,24 +1725,24 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="23"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
       <c r="L27" s="7">
         <v>44736</v>
       </c>
@@ -1754,24 +1754,24 @@
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="5" t="s">
         <v>67</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
       <c r="L28" s="7">
         <v>44736</v>
       </c>
@@ -1783,24 +1783,24 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="5" t="s">
         <v>70</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="23"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="7">
         <v>44736</v>
       </c>
@@ -1812,24 +1812,24 @@
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="25" t="s">
+      <c r="H30" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="23"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
       <c r="L30" s="7">
         <v>44748</v>
       </c>
@@ -1841,24 +1841,24 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="23"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="22"/>
       <c r="L31" s="7">
         <v>44755</v>
       </c>
@@ -1871,18 +1871,18 @@
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="23"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="12">
         <f>L25</f>
         <v>44736</v>
@@ -1896,24 +1896,24 @@
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="23"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="23"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="22"/>
       <c r="L33" s="8">
         <f>M32</f>
         <v>44757</v>
@@ -1926,24 +1926,24 @@
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="23"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="23"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="22"/>
       <c r="L34" s="7">
         <v>44757</v>
       </c>
@@ -1955,24 +1955,24 @@
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="23"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="22"/>
       <c r="L35" s="7">
         <v>44757</v>
       </c>
@@ -1984,24 +1984,24 @@
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="23"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="23"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="22"/>
       <c r="L36" s="7">
         <v>44757</v>
       </c>
@@ -2013,24 +2013,24 @@
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="23"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H37" s="25" t="s">
+      <c r="H37" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="23"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="22"/>
       <c r="L37" s="7">
         <v>44757</v>
       </c>
@@ -2042,24 +2042,24 @@
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="23"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22"/>
       <c r="F38" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="25" t="s">
+      <c r="H38" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="23"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="22"/>
       <c r="L38" s="7">
         <v>44762</v>
       </c>
@@ -2071,24 +2071,24 @@
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="23"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
       <c r="F39" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="23"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="22"/>
       <c r="L39" s="7">
         <v>44762</v>
       </c>
@@ -2100,24 +2100,24 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
       <c r="F40" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="23"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="22"/>
       <c r="L40" s="7">
         <v>44764</v>
       </c>
@@ -2129,24 +2129,24 @@
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
       <c r="F41" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="25" t="s">
+      <c r="H41" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="23"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="22"/>
       <c r="L41" s="7">
         <v>44769</v>
       </c>
@@ -2158,24 +2158,24 @@
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
       <c r="F42" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="23"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="22"/>
       <c r="L42" s="7">
         <v>44769</v>
       </c>
@@ -2187,24 +2187,24 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="23"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
       <c r="F43" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="23"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="22"/>
       <c r="L43" s="7">
         <v>44777</v>
       </c>
@@ -2216,24 +2216,24 @@
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="22"/>
       <c r="F44" s="5" t="s">
         <v>100</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H44" s="25" t="s">
+      <c r="H44" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="23"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="22"/>
       <c r="L44" s="7">
         <v>44777</v>
       </c>
@@ -2245,18 +2245,18 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="36"/>
       <c r="F45" s="15"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="29"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="36"/>
       <c r="L45" s="17">
         <f>L33</f>
         <v>44757</v>
@@ -2270,14 +2270,14 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G47" s="1"/>
@@ -5146,45 +5146,38 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H40:K40"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
@@ -5201,38 +5194,45 @@
     <mergeCell ref="H44:K44"/>
     <mergeCell ref="H32:K32"/>
     <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5253,120 +5253,120 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="41" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="41" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="41" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="41" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="41" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="41" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F11" s="2"/>
@@ -5392,13 +5392,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:H10"/>
@@ -5414,6 +5407,13 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>